<commit_message>
add map and fix edit part
</commit_message>
<xml_diff>
--- a/xlsx/export.xlsx
+++ b/xlsx/export.xlsx
@@ -5,10 +5,10 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EXT03426951\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EXT03426951\Desktop\extension-for-envanter\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AEDFACE-393D-4025-9EC5-258F5E16D4E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71470C47-54BC-426D-B7EE-23B64912F7B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -951,9 +951,6 @@
     <t>08 Mayıs 2025 16:13:00</t>
   </si>
   <si>
-    <t>SERİVS ETKİSİ</t>
-  </si>
-  <si>
     <t>AYBER;BUBSC;MEKZY;SANGR</t>
   </si>
   <si>
@@ -1059,6 +1056,9 @@
   </si>
   <si>
     <t>Arıza Süresi</t>
+  </si>
+  <si>
+    <t>Etkilenen Servis Bilgileri</t>
   </si>
 </sst>
 </file>
@@ -1199,11 +1199,11 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1521,8 +1521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I66" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="U72" sqref="U72"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6328125" defaultRowHeight="60" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1530,11 +1530,11 @@
     <col min="1" max="2" width="10.6328125" style="4"/>
     <col min="3" max="4" width="15.6328125" style="4" customWidth="1"/>
     <col min="5" max="5" width="30.6328125" style="4" customWidth="1"/>
-    <col min="6" max="7" width="10.6328125" style="13"/>
-    <col min="8" max="8" width="20.6328125" style="13" customWidth="1"/>
+    <col min="6" max="7" width="10.6328125" style="4"/>
+    <col min="8" max="8" width="16.81640625" style="4" customWidth="1"/>
     <col min="9" max="9" width="10.6328125" style="4"/>
     <col min="10" max="11" width="15.6328125" style="4" customWidth="1"/>
-    <col min="12" max="14" width="10.6328125" style="13"/>
+    <col min="12" max="14" width="10.6328125" style="4"/>
     <col min="15" max="16" width="20.6328125" style="4" customWidth="1"/>
     <col min="17" max="21" width="10.6328125" style="4"/>
     <col min="22" max="22" width="20.6328125" style="4" customWidth="1"/>
@@ -1559,13 +1559,13 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>305</v>
+      <c r="H1" s="14" t="s">
+        <v>332</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>5</v>
@@ -1577,13 +1577,13 @@
         <v>7</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="M1" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>309</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>310</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>8</v>
@@ -1601,16 +1601,16 @@
         <v>12</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="W1" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="60" customHeight="1" x14ac:dyDescent="0.35">
@@ -5181,16 +5181,16 @@
         <v>297</v>
       </c>
       <c r="F69" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="G69" s="12" t="s">
         <v>316</v>
       </c>
-      <c r="G69" s="12" t="s">
-        <v>317</v>
-      </c>
       <c r="H69" s="12" t="s">
+        <v>305</v>
+      </c>
+      <c r="I69" s="10" t="s">
         <v>306</v>
-      </c>
-      <c r="I69" s="10" t="s">
-        <v>307</v>
       </c>
       <c r="J69" s="10" t="s">
         <v>298</v>
@@ -5214,7 +5214,7 @@
         <v>156</v>
       </c>
       <c r="Q69" s="8" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="R69" s="8" t="s">
         <v>24</v>
@@ -5223,16 +5223,16 @@
         <v>81</v>
       </c>
       <c r="T69" s="8" t="s">
-        <v>324</v>
-      </c>
-      <c r="U69" s="14" t="s">
-        <v>324</v>
+        <v>323</v>
+      </c>
+      <c r="U69" s="13" t="s">
+        <v>323</v>
       </c>
       <c r="V69" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="W69" s="3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="70" spans="1:23" ht="60" customHeight="1" x14ac:dyDescent="0.35">
@@ -5252,14 +5252,14 @@
         <v>38</v>
       </c>
       <c r="F70" s="12" t="s">
+        <v>317</v>
+      </c>
+      <c r="G70" s="12" t="s">
         <v>318</v>
-      </c>
-      <c r="G70" s="12" t="s">
-        <v>319</v>
       </c>
       <c r="H70" s="12"/>
       <c r="I70" s="10" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="J70" s="10" t="s">
         <v>300</v>
@@ -5268,7 +5268,7 @@
         <v>301</v>
       </c>
       <c r="L70" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="M70" s="12">
         <v>327</v>
@@ -5283,7 +5283,7 @@
         <v>302</v>
       </c>
       <c r="Q70" s="8" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="R70" s="8" t="s">
         <v>24</v>
@@ -5292,16 +5292,16 @@
         <v>24</v>
       </c>
       <c r="T70" s="8" t="s">
-        <v>313</v>
-      </c>
-      <c r="U70" s="14" t="s">
-        <v>313</v>
+        <v>312</v>
+      </c>
+      <c r="U70" s="13" t="s">
+        <v>312</v>
       </c>
       <c r="V70" s="3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="W70" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="71" spans="1:23" ht="60" customHeight="1" x14ac:dyDescent="0.35">
@@ -5321,14 +5321,14 @@
         <v>235</v>
       </c>
       <c r="F71" s="12" t="s">
+        <v>319</v>
+      </c>
+      <c r="G71" s="12" t="s">
         <v>320</v>
-      </c>
-      <c r="G71" s="12" t="s">
-        <v>321</v>
       </c>
       <c r="H71" s="12"/>
       <c r="I71" s="10" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="J71" s="10" t="s">
         <v>303</v>
@@ -5352,25 +5352,25 @@
         <v>287</v>
       </c>
       <c r="Q71" s="8" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="R71" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="S71" s="8" t="s">
         <v>24</v>
       </c>
       <c r="T71" s="8" t="s">
-        <v>313</v>
-      </c>
-      <c r="U71" s="14" t="s">
-        <v>313</v>
+        <v>312</v>
+      </c>
+      <c r="U71" s="13" t="s">
+        <v>312</v>
       </c>
       <c r="V71" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="W71" s="3" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
readme uploaded, next.. r1 llm entegration
</commit_message>
<xml_diff>
--- a/xlsx/export.xlsx
+++ b/xlsx/export.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EXT03426951\Desktop\extension-for-envanter\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA6ED26A-4F2A-496E-A5B3-250845EDECDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6339C5C3-EB64-4622-B0E0-E075AE865A75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="826" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="826" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fiber Arıza" sheetId="1" r:id="rId1"/>
@@ -1651,7 +1651,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB71"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
@@ -5899,7 +5899,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0E91290-0C96-4C80-BCA2-F97D6D5A5CAA}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="I2" sqref="I2:I3"/>
     </sheetView>
   </sheetViews>

</xml_diff>